<commit_message>
Working on tests for S5_Shear.
</commit_message>
<xml_diff>
--- a/tests/Excel/AS4100_5_Shear Verification.xlsx
+++ b/tests/Excel/AS4100_5_Shear Verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seank\PycharmProjects\BeamDesign\tests\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DCC9D0-2242-43EF-A146-FEED9763F2E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150282D0-9AB6-463D-8FC2-D77749122B0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1835,8 +1835,8 @@
     <numFmt numFmtId="181" formatCode="##0.00E+00&quot; N&quot;"/>
     <numFmt numFmtId="182" formatCode="##0.00E+00&quot; Pa&quot;"/>
     <numFmt numFmtId="183" formatCode="0&quot; kg/m&quot;"/>
-    <numFmt numFmtId="187" formatCode="0.000&quot; m²&quot;"/>
-    <numFmt numFmtId="188" formatCode="##0.00E+00&quot; m³&quot;"/>
+    <numFmt numFmtId="184" formatCode="0.000&quot; m²&quot;"/>
+    <numFmt numFmtId="185" formatCode="##0.00E+00&quot; m³&quot;"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -2094,9 +2094,9 @@
     <xf numFmtId="183" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="184" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="178" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="188" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="185" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="179" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2107,221 +2107,6 @@
   <dxfs count="243">
     <dxf>
       <numFmt numFmtId="181" formatCode="##0.00E+00&quot; N&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="180" formatCode="##0E+00&quot; Pa&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="179" formatCode="##0.00E+00&quot; m⁶&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="188" formatCode="##0.00E+00&quot; m³&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="188" formatCode="##0.00E+00&quot; m³&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="188" formatCode="##0.00E+00&quot; m³&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="188" formatCode="##0.00E+00&quot; m³&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="187" formatCode="0.000&quot; m²&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="183" formatCode="0&quot; kg/m&quot;"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6728,6 +6513,221 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="180" formatCode="##0E+00&quot; Pa&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="179" formatCode="##0.00E+00&quot; m⁶&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="185" formatCode="##0.00E+00&quot; m³&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="185" formatCode="##0.00E+00&quot; m³&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="185" formatCode="##0.00E+00&quot; m³&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="185" formatCode="##0.00E+00&quot; m³&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="##0.00E+00&quot; m⁴&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="184" formatCode="0.000&quot; m²&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000&quot; m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="183" formatCode="0&quot; kg/m&quot;"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFF0F0F4"/>
@@ -6798,35 +6798,35 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDDEE4D4-895F-4D98-BD2B-A1595D136FE1}" name="Table8" displayName="Table8" ref="B2:AA25" totalsRowShown="0">
   <autoFilter ref="B2:AA25" xr:uid="{0AC04653-982D-4DB0-97C0-530DC6DA1D7C}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{280EAB9D-68EA-4683-A885-68F041F7C696}" name="Section" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{607776AD-1CEA-4ABA-9EBB-6E7242760D55}" name="Designation" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{8B64A8C3-F92A-47F9-96F3-AA3D2FB57C71}" name="Mass" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{C3F54EAF-B082-4E92-89A4-EB922C48C2FD}" name="Section Type" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{099E95F4-155C-46BC-9B68-09B5DC82AC9E}" name="Fabrication Type" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{603611E8-32D2-418A-B7F1-7978728F31CE}" name="d" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{8C2BF6A8-8480-4D0B-8189-8DD35F84F37A}" name="bf" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{AF33BA8F-44DE-4FA5-B937-5086CFDD19FF}" name="tf" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{688540C0-5BD0-4CE3-8BC7-7345CE0E5749}" name="tw" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{1C612196-CED2-42B0-865A-D4E03216B7B7}" name="d1" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{4F3DA98F-ED30-4ACB-A515-75F8C0DC4843}" name="d1 / tw" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{22B64CBB-F443-44A9-9500-7B9BBDFB124B}" name="(bf - tw) / (2 × tf)" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{D4DF694A-4484-4C9F-9376-6A57C15AF617}" name="Ag" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{3724EE49-662E-4E0E-A37B-3ADE156496AD}" name="Ix" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{AD4648AD-343E-4A35-9246-69098C5044CC}" name="Zx" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{0ABFCF14-5F21-419A-9559-2CA91A10474B}" name="Sx" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{DC4F87E0-E5C6-4D73-A757-8F63BAF7554D}" name="rx" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{23E1E09C-910E-46AB-90C7-90D38D81B99E}" name="Iy" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{885B4339-7E0D-4B91-9FC6-5D81E2299F9C}" name="Zy" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{84C35746-536E-4B01-8256-14A9DCAB142B}" name="Sy" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{A7686837-B7AE-4BAE-88E2-6F9FAD730E01}" name="ry" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{767ED161-3BD1-4294-96E7-EF008EBAF27A}" name="J" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{4874CB8A-E902-4CEB-AEFF-C3681E512597}" name="Iw" dataDxfId="2"/>
-    <tableColumn id="26" xr3:uid="{4B448337-5DAD-4159-85BB-146825F8C228}" name="fy" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{473325F2-FF03-4C75-BD12-A70F0A6AA4F1}" name="Aw" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{280EAB9D-68EA-4683-A885-68F041F7C696}" name="Section" dataDxfId="239"/>
+    <tableColumn id="2" xr3:uid="{607776AD-1CEA-4ABA-9EBB-6E7242760D55}" name="Designation" dataDxfId="238"/>
+    <tableColumn id="3" xr3:uid="{8B64A8C3-F92A-47F9-96F3-AA3D2FB57C71}" name="Mass" dataDxfId="237"/>
+    <tableColumn id="4" xr3:uid="{C3F54EAF-B082-4E92-89A4-EB922C48C2FD}" name="Section Type" dataDxfId="236"/>
+    <tableColumn id="5" xr3:uid="{099E95F4-155C-46BC-9B68-09B5DC82AC9E}" name="Fabrication Type" dataDxfId="235"/>
+    <tableColumn id="6" xr3:uid="{603611E8-32D2-418A-B7F1-7978728F31CE}" name="d" dataDxfId="234"/>
+    <tableColumn id="7" xr3:uid="{8C2BF6A8-8480-4D0B-8189-8DD35F84F37A}" name="bf" dataDxfId="233"/>
+    <tableColumn id="8" xr3:uid="{AF33BA8F-44DE-4FA5-B937-5086CFDD19FF}" name="tf" dataDxfId="232"/>
+    <tableColumn id="9" xr3:uid="{688540C0-5BD0-4CE3-8BC7-7345CE0E5749}" name="tw" dataDxfId="231"/>
+    <tableColumn id="10" xr3:uid="{1C612196-CED2-42B0-865A-D4E03216B7B7}" name="d1" dataDxfId="230"/>
+    <tableColumn id="11" xr3:uid="{4F3DA98F-ED30-4ACB-A515-75F8C0DC4843}" name="d1 / tw" dataDxfId="229"/>
+    <tableColumn id="12" xr3:uid="{22B64CBB-F443-44A9-9500-7B9BBDFB124B}" name="(bf - tw) / (2 × tf)" dataDxfId="228"/>
+    <tableColumn id="13" xr3:uid="{D4DF694A-4484-4C9F-9376-6A57C15AF617}" name="Ag" dataDxfId="227"/>
+    <tableColumn id="14" xr3:uid="{3724EE49-662E-4E0E-A37B-3ADE156496AD}" name="Ix" dataDxfId="226"/>
+    <tableColumn id="15" xr3:uid="{AD4648AD-343E-4A35-9246-69098C5044CC}" name="Zx" dataDxfId="225"/>
+    <tableColumn id="16" xr3:uid="{0ABFCF14-5F21-419A-9559-2CA91A10474B}" name="Sx" dataDxfId="224"/>
+    <tableColumn id="17" xr3:uid="{DC4F87E0-E5C6-4D73-A757-8F63BAF7554D}" name="rx" dataDxfId="223"/>
+    <tableColumn id="18" xr3:uid="{23E1E09C-910E-46AB-90C7-90D38D81B99E}" name="Iy" dataDxfId="222"/>
+    <tableColumn id="19" xr3:uid="{885B4339-7E0D-4B91-9FC6-5D81E2299F9C}" name="Zy" dataDxfId="221"/>
+    <tableColumn id="20" xr3:uid="{84C35746-536E-4B01-8256-14A9DCAB142B}" name="Sy" dataDxfId="220"/>
+    <tableColumn id="21" xr3:uid="{A7686837-B7AE-4BAE-88E2-6F9FAD730E01}" name="ry" dataDxfId="219"/>
+    <tableColumn id="22" xr3:uid="{767ED161-3BD1-4294-96E7-EF008EBAF27A}" name="J" dataDxfId="218"/>
+    <tableColumn id="23" xr3:uid="{4874CB8A-E902-4CEB-AEFF-C3681E512597}" name="Iw" dataDxfId="217"/>
+    <tableColumn id="26" xr3:uid="{4B448337-5DAD-4159-85BB-146825F8C228}" name="fy" dataDxfId="216"/>
+    <tableColumn id="24" xr3:uid="{473325F2-FF03-4C75-BD12-A70F0A6AA4F1}" name="Aw" dataDxfId="215">
       <calculatedColumnFormula>Table8[[#This Row],[d1]]*Table8[[#This Row],[tw]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="25" xr3:uid="{98B29A8D-CA7E-401A-9966-485A14A8FF27}" name="φVyield" dataDxfId="0">
-      <calculatedColumnFormula>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</calculatedColumnFormula>
+      <calculatedColumnFormula>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6834,45 +6834,45 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblEuler" displayName="tblEuler" ref="B2:AA57" totalsRowShown="0" headerRowDxfId="239" dataDxfId="238">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblEuler" displayName="tblEuler" ref="B2:AA57" totalsRowShown="0" headerRowDxfId="214" dataDxfId="213">
   <autoFilter ref="B2:AA57" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Section" dataDxfId="237"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="An" dataDxfId="236"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="kf" dataDxfId="235"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="lex" dataDxfId="234"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ley" dataDxfId="233"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="lez" dataDxfId="232"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="rx" dataDxfId="231"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ry" dataDxfId="230"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="xo" dataDxfId="229"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="yo" dataDxfId="228"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Ix" dataDxfId="227"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Iy" dataDxfId="226"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="J" dataDxfId="225"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Iw" dataDxfId="224"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="fy" dataDxfId="223"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="E" dataDxfId="222"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="G" dataDxfId="221"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="fref" dataDxfId="220"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="αb" dataDxfId="219"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Axis" dataDxfId="218"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="feuler_x" dataDxfId="217">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Section" dataDxfId="212"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="An" dataDxfId="211"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="kf" dataDxfId="210"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="lex" dataDxfId="209"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ley" dataDxfId="208"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="lez" dataDxfId="207"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="rx" dataDxfId="206"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ry" dataDxfId="205"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="xo" dataDxfId="204"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="yo" dataDxfId="203"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Ix" dataDxfId="202"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Iy" dataDxfId="201"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="J" dataDxfId="200"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Iw" dataDxfId="199"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="fy" dataDxfId="198"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="E" dataDxfId="197"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="G" dataDxfId="196"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="fref" dataDxfId="195"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="αb" dataDxfId="194"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Axis" dataDxfId="193"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="feuler_x" dataDxfId="192">
       <calculatedColumnFormula>(tblEuler[[#This Row],[E]]*PI()^2)/((tblEuler[[#This Row],[lex]]/tblEuler[[#This Row],[rx]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Neuler_x" dataDxfId="216">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Neuler_x" dataDxfId="191">
       <calculatedColumnFormula>(tblEuler[[#This Row],[Ix]]*tblEuler[[#This Row],[E]]*PI()^2)/(tblEuler[[#This Row],[lex]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Feuler_y" dataDxfId="215">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Feuler_y" dataDxfId="190">
       <calculatedColumnFormula>(tblEuler[[#This Row],[E]]*PI()^2)/((tblEuler[[#This Row],[ley]]/tblEuler[[#This Row],[ry]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Neuler_y" dataDxfId="214">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Neuler_y" dataDxfId="189">
       <calculatedColumnFormula>(tblEuler[[#This Row],[Iy]]*tblEuler[[#This Row],[E]]*PI()^2)/(tblEuler[[#This Row],[ley]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="rol" dataDxfId="213">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="rol" dataDxfId="188">
       <calculatedColumnFormula>SQRT(tblEuler[[#This Row],[rx]]^2+tblEuler[[#This Row],[ry]]^2+tblEuler[[#This Row],[xo]]^2+tblEuler[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Feuler_torsion" dataDxfId="212">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Feuler_torsion" dataDxfId="187">
       <calculatedColumnFormula>((tblEuler[[#This Row],[G]]*tblEuler[[#This Row],[J]])/(tblEuler[[#This Row],[An]]*tblEuler[[#This Row],[rol]]^2))*(1+((tblEuler[[#This Row],[Iw]]*tblEuler[[#This Row],[E]]*PI()^2)/(tblEuler[[#This Row],[G]]*tblEuler[[#This Row],[J]]*tblEuler[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6881,127 +6881,127 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblNc" displayName="tblNc" ref="B3:BB58" totalsRowShown="0" headerRowDxfId="211" dataDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblNc" displayName="tblNc" ref="B3:BB58" totalsRowShown="0" headerRowDxfId="186" dataDxfId="185">
   <autoFilter ref="B3:BB58" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:AL58">
     <sortCondition ref="B3:B58"/>
   </sortState>
   <tableColumns count="53">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Section" dataDxfId="209"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="An" dataDxfId="208"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="kf" dataDxfId="207"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="l" dataDxfId="206"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="kex" dataDxfId="205"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="key" dataDxfId="204"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0100-000030000000}" name="kez" dataDxfId="203"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="rx" dataDxfId="202"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ry" dataDxfId="201"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="xo" dataDxfId="200"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="yo" dataDxfId="199"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="J" dataDxfId="198"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="Iw" dataDxfId="197"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="fy" dataDxfId="196"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="E" dataDxfId="195"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="G" dataDxfId="194"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="fref" dataDxfId="193"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="αb" dataDxfId="192"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="Axis" dataDxfId="191"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0100-00002F000000}" name="calc_buckle" dataDxfId="190"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0100-00002E000000}" name="calc_torsion" dataDxfId="189"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Ae" dataDxfId="188">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Section" dataDxfId="184"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="An" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="kf" dataDxfId="182"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0100-000033000000}" name="l" dataDxfId="181"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0100-000032000000}" name="kex" dataDxfId="180"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0100-000031000000}" name="key" dataDxfId="179"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0100-000030000000}" name="kez" dataDxfId="178"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="rx" dataDxfId="177"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ry" dataDxfId="176"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="xo" dataDxfId="175"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="yo" dataDxfId="174"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="J" dataDxfId="173"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="Iw" dataDxfId="172"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="fy" dataDxfId="171"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="E" dataDxfId="170"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="G" dataDxfId="169"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="fref" dataDxfId="168"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="αb" dataDxfId="167"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="Axis" dataDxfId="166"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0100-00002F000000}" name="calc_buckle" dataDxfId="165"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0100-00002E000000}" name="calc_torsion" dataDxfId="164"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="Ae" dataDxfId="163">
       <calculatedColumnFormula>tblNc[[#This Row],[An]]*tblNc[[#This Row],[kf]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ns" dataDxfId="187">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="Ns" dataDxfId="162">
       <calculatedColumnFormula>tblNc[[#This Row],[Ae]]*tblNc[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="φNs" dataDxfId="186">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="φNs" dataDxfId="161">
       <calculatedColumnFormula>tblNc[[#This Row],[Ns]]*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="lex" dataDxfId="185">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="lex" dataDxfId="160">
       <calculatedColumnFormula>tblNc[[#This Row],[l]]*tblNc[[#This Row],[kex]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="ley" dataDxfId="184">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="ley" dataDxfId="159">
       <calculatedColumnFormula>tblNc[[#This Row],[l]]*tblNc[[#This Row],[key]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="lez" dataDxfId="183">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="lez" dataDxfId="158">
       <calculatedColumnFormula>tblNc[[#This Row],[kez]]*tblNc[[#This Row],[l]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="λnx" dataDxfId="182">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="λnx" dataDxfId="157">
       <calculatedColumnFormula>(tblNc[[#This Row],[lex]]/tblNc[[#This Row],[rx]])*(SQRT(tblNc[[#This Row],[kf]]))*SQRT((tblNc[[#This Row],[fy]]/tblNc[[#This Row],[fref]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="αax" dataDxfId="181">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="αax" dataDxfId="156">
       <calculatedColumnFormula>(2100*(tblNc[[#This Row],[λnx]]-13.5))/((tblNc[[#This Row],[λnx]]^2)-(15.3*tblNc[[#This Row],[λnx]])+2050)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="λx" dataDxfId="180">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="λx" dataDxfId="155">
       <calculatedColumnFormula>tblNc[[#This Row],[λnx]]+tblNc[[#This Row],[αax]]*tblNc[[#This Row],[αb]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="ηx" dataDxfId="179">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="ηx" dataDxfId="154">
       <calculatedColumnFormula>MAX((0.00326*(tblNc[[#This Row],[λx]]-13.5)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="ξx" dataDxfId="178">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="ξx" dataDxfId="153">
       <calculatedColumnFormula>((tblNc[[#This Row],[λx]]/90)^2+1+tblNc[[#This Row],[ηx]])/(2*(tblNc[[#This Row],[λx]]/90)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="αcx" dataDxfId="177">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="αcx" dataDxfId="152">
       <calculatedColumnFormula>tblNc[[#This Row],[ξx]]*(1-SQRT(1-(90/(tblNc[[#This Row],[ξx]]*tblNc[[#This Row],[λx]]))^2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="Ncx" dataDxfId="176">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="Ncx" dataDxfId="151">
       <calculatedColumnFormula>tblNc[[#This Row],[αcx]]*tblNc[[#This Row],[Ns]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="φNcx" dataDxfId="175">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0100-000035000000}" name="φNcx" dataDxfId="150">
       <calculatedColumnFormula>tblNc[[#This Row],[Ncx]]*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="λny" dataDxfId="174">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="λny" dataDxfId="149">
       <calculatedColumnFormula>(tblNc[[#This Row],[lex]]/tblNc[[#This Row],[ry]])*(SQRT(tblNc[[#This Row],[kf]]))*SQRT((tblNc[[#This Row],[fy]]/tblNc[[#This Row],[fref]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="αay" dataDxfId="173">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="αay" dataDxfId="148">
       <calculatedColumnFormula>(2100*(tblNc[[#This Row],[λny]]-13.5))/((tblNc[[#This Row],[λny]]^2)-(15.3*tblNc[[#This Row],[λny]])+2050)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="λy" dataDxfId="172">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="λy" dataDxfId="147">
       <calculatedColumnFormula>tblNc[[#This Row],[λny]]+tblNc[[#This Row],[αay]]*tblNc[[#This Row],[αb]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="ηy" dataDxfId="171">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="ηy" dataDxfId="146">
       <calculatedColumnFormula>MAX((0.00326*(tblNc[[#This Row],[λy]]-13.5)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="ξy" dataDxfId="170">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="ξy" dataDxfId="145">
       <calculatedColumnFormula>((tblNc[[#This Row],[λy]]/90)^2+1+tblNc[[#This Row],[ηy]])/(2*(tblNc[[#This Row],[λy]]/90)^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="αcy" dataDxfId="169">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="αcy" dataDxfId="144">
       <calculatedColumnFormula>tblNc[[#This Row],[ξy]]*(1-SQRT(1-(90/(tblNc[[#This Row],[ξy]]*tblNc[[#This Row],[λy]]))^2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Ncy" dataDxfId="168">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Ncy" dataDxfId="143">
       <calculatedColumnFormula>tblNc[[#This Row],[αcy]]*tblNc[[#This Row],[Ns]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="φNcy" dataDxfId="167">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0100-000034000000}" name="φNcy" dataDxfId="142">
       <calculatedColumnFormula>tblNc[[#This Row],[Ncy]]*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Ncflex" dataDxfId="166">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Ncflex" dataDxfId="141">
       <calculatedColumnFormula>MIN(tblNc[[#This Row],[Ncy]],tblNc[[#This Row],[Ncx]],tblNc[[#This Row],[Ns]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="φNcflex" dataDxfId="165">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="φNcflex" dataDxfId="140">
       <calculatedColumnFormula>tblNc[[#This Row],[Ncflex]]*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="Ncz_dbl" dataDxfId="164">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="Ncz_dbl" dataDxfId="139">
       <calculatedColumnFormula array="1">INDEX(tblfocDblSym[Nc],MATCH(tblNc[[#This Row],[Section]]&amp;tblNc[[#This Row],[lex]],tblfocDblSym[Section]&amp;tblfocDblSym[lex],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="Ncz_sngl" dataDxfId="163">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="Ncz_sngl" dataDxfId="138">
       <calculatedColumnFormula array="1">INDEX(tblfocSglSym[Nc],MATCH(tblNc[[#This Row],[Section]]&amp;tblNc[[#This Row],[lex]],tblfocSglSym[Section]&amp;tblfocSglSym[lex],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="Ncz_un" dataDxfId="162">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="Ncz_un" dataDxfId="137">
       <calculatedColumnFormula array="1">INDEX(tblfocunsym[Nc],MATCH(tblNc[[#This Row],[Section]]&amp;tblNc[[#This Row],[lex]],tblfocunsym[Section]&amp;tblfocunsym[lex],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="Ncz_base" dataDxfId="161">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name="Ncz_base" dataDxfId="136">
       <calculatedColumnFormula>IF(tblNc[[#This Row],[Axis]]="['x', 'y']",tblNc[[#This Row],[Ncz_dbl]],IF(tblNc[[#This Row],[Axis]]="[]",tblNc[[#This Row],[Ncz_un]],tblNc[[#This Row],[Ncz_sngl]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="Ncz" dataDxfId="160">
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="Ncz" dataDxfId="135">
       <calculatedColumnFormula>MIN(tblNc[[#This Row],[Ncz_base]],tblNc[[#This Row],[Ns]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="φNcz" dataDxfId="159">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="φNcz" dataDxfId="134">
       <calculatedColumnFormula>tblNc[[#This Row],[Ncz]]*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Nc" dataDxfId="158">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="Nc" dataDxfId="133">
       <calculatedColumnFormula>MIN(tblNc[[#This Row],[Ncflex]],tblNc[[#This Row],[Ncz]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="φNc" dataDxfId="157">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="φNc" dataDxfId="132">
       <calculatedColumnFormula>tblNc[[#This Row],[Nc]]*0.9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7010,34 +7010,34 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblfoxz" displayName="tblfoxz" ref="B2:R57" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tblfoxz" displayName="tblfoxz" ref="B2:R57" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <autoFilter ref="B2:R57" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Section" dataDxfId="154"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="An" dataDxfId="153"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="lex" dataDxfId="152"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="lez" dataDxfId="151"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="rx" dataDxfId="150"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="ry" dataDxfId="149"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="xo" dataDxfId="148"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="yo" dataDxfId="147"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="J" dataDxfId="146"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Iw" dataDxfId="145"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="E" dataDxfId="144"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="G" dataDxfId="143"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="rol" dataDxfId="142">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Section" dataDxfId="129"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="An" dataDxfId="128"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="lex" dataDxfId="127"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="lez" dataDxfId="126"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="rx" dataDxfId="125"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="ry" dataDxfId="124"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="xo" dataDxfId="123"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="yo" dataDxfId="122"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="J" dataDxfId="121"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Iw" dataDxfId="120"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="E" dataDxfId="119"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="G" dataDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="rol" dataDxfId="117">
       <calculatedColumnFormula>SQRT(tblfoxz[[#This Row],[rx]]^2+tblfoxz[[#This Row],[ry]]^2+tblfoxz[[#This Row],[xo]]^2+tblfoxz[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="fox" dataDxfId="141">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="fox" dataDxfId="116">
       <calculatedColumnFormula>(tblfoxz[[#This Row],[E]]*PI()^2)/((tblfoxz[[#This Row],[lex]]/tblfoxz[[#This Row],[rx]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="foz" dataDxfId="140">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="foz" dataDxfId="115">
       <calculatedColumnFormula>((tblfoxz[[#This Row],[G]]*tblfoxz[[#This Row],[J]])/(tblfoxz[[#This Row],[An]]*tblfoxz[[#This Row],[rol]]^2))*(1+((tblfoxz[[#This Row],[Iw]]*tblfoxz[[#This Row],[E]]*PI()^2)/(tblfoxz[[#This Row],[G]]*tblfoxz[[#This Row],[J]]*tblfoxz[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="β" dataDxfId="139">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="β" dataDxfId="114">
       <calculatedColumnFormula>1-(tblfoxz[[#This Row],[xo]]/tblfoxz[[#This Row],[rol]])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="f_oxz" dataDxfId="138">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="f_oxz" dataDxfId="113">
       <calculatedColumnFormula>(1/(2*tblfoxz[[#This Row],[β]]))*((tblfoxz[[#This Row],[fox]]+tblfoxz[[#This Row],[foz]])-SQRT((tblfoxz[[#This Row],[fox]]+tblfoxz[[#This Row],[foz]])^2-4*tblfoxz[[#This Row],[β]]*tblfoxz[[#This Row],[fox]]*tblfoxz[[#This Row],[foz]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7046,50 +7046,50 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblfocDblSym" displayName="tblfocDblSym" ref="B2:Z22" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tblfocDblSym" displayName="tblfocDblSym" ref="B2:Z22" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
   <autoFilter ref="B2:Z22" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Section" dataDxfId="135"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="An" dataDxfId="134"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0300-000017000000}" name="kf" dataDxfId="133"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="lex" dataDxfId="132"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0300-000019000000}" name="ley" dataDxfId="131"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="lez" dataDxfId="130"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="rx" dataDxfId="129"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="ry" dataDxfId="128"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="xo" dataDxfId="127"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="yo" dataDxfId="126"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="J" dataDxfId="125"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="Iw" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="fy" dataDxfId="123"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="E" dataDxfId="122"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="G" dataDxfId="121"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0300-000018000000}" name="Axis" dataDxfId="120"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="rol" dataDxfId="119">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Section" dataDxfId="110"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="An" dataDxfId="109"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0300-000017000000}" name="kf" dataDxfId="108"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0300-00000E000000}" name="lex" dataDxfId="107"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0300-000019000000}" name="ley" dataDxfId="106"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0300-000013000000}" name="lez" dataDxfId="105"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="rx" dataDxfId="104"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="ry" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="xo" dataDxfId="102"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="yo" dataDxfId="101"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="J" dataDxfId="100"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0300-000014000000}" name="Iw" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="fy" dataDxfId="98"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="E" dataDxfId="97"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="G" dataDxfId="96"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0300-000018000000}" name="Axis" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="rol" dataDxfId="94">
       <calculatedColumnFormula>SQRT(tblfocDblSym[[#This Row],[rx]]^2+tblfocDblSym[[#This Row],[ry]]^2+tblfocDblSym[[#This Row],[xo]]^2+tblfocDblSym[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="fox" dataDxfId="118">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="fox" dataDxfId="93">
       <calculatedColumnFormula>(tblfocDblSym[[#This Row],[E]]*PI()^2)/((tblfocDblSym[[#This Row],[lex]]/tblfocDblSym[[#This Row],[rx]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="foz" dataDxfId="117">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="foz" dataDxfId="92">
       <calculatedColumnFormula>((tblfocDblSym[[#This Row],[G]]*tblfocDblSym[[#This Row],[J]])/(tblfocDblSym[[#This Row],[An]]*tblfocDblSym[[#This Row],[rol]]^2))*(1+((tblfocDblSym[[#This Row],[Iw]]*tblfocDblSym[[#This Row],[E]]*PI()^2)/(tblfocDblSym[[#This Row],[G]]*tblfocDblSym[[#This Row],[J]]*tblfocDblSym[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="β" dataDxfId="116">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="β" dataDxfId="91">
       <calculatedColumnFormula>1-(tblfocDblSym[[#This Row],[xo]]/tblfocDblSym[[#This Row],[rol]])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="foxz" dataDxfId="115">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="foxz" dataDxfId="90">
       <calculatedColumnFormula>(1/(2*tblfocDblSym[[#This Row],[β]]))*((tblfocDblSym[[#This Row],[fox]]+tblfocDblSym[[#This Row],[foz]])-SQRT((tblfocDblSym[[#This Row],[fox]]+tblfocDblSym[[#This Row],[foz]])^2-4*tblfocDblSym[[#This Row],[β]]*tblfocDblSym[[#This Row],[fox]]*tblfocDblSym[[#This Row],[foz]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="foc" dataDxfId="114">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0300-000015000000}" name="foc" dataDxfId="89">
       <calculatedColumnFormula>MIN(tblfocDblSym[[#This Row],[foxz]],tblfocDblSym[[#This Row],[foz]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="λc" dataDxfId="113">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="λc" dataDxfId="88">
       <calculatedColumnFormula>SQRT(tblfocDblSym[[#This Row],[fy]]/tblfocDblSym[[#This Row],[foc]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="fn" dataDxfId="112">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0300-00000F000000}" name="fn" dataDxfId="87">
       <calculatedColumnFormula>IF(tblfocDblSym[[#This Row],[λc]]&lt;=1.5,0.658^(tblfocDblSym[[#This Row],[λc]]^2),0.877/(tblfocDblSym[[#This Row],[λc]]^2))*tblfocDblSym[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0300-000016000000}" name="Nc" dataDxfId="111">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0300-000016000000}" name="Nc" dataDxfId="86">
       <calculatedColumnFormula>0.85*tblfocDblSym[[#This Row],[An]]*tblfocDblSym[[#This Row],[kf]]*tblfocDblSym[[#This Row],[fn]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7098,62 +7098,62 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblfocSglSym" displayName="tblfocSglSym" ref="B2:AC31" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tblfocSglSym" displayName="tblfocSglSym" ref="B2:AC31" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
   <autoFilter ref="B2:AC31" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:AC31">
     <sortCondition ref="B2:B31"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Section" dataDxfId="108"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="An" dataDxfId="107"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="kf" dataDxfId="106"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="lex" dataDxfId="105"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="ley" dataDxfId="104"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="lez" dataDxfId="103"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="rx" dataDxfId="102"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="ry" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="xo" dataDxfId="100"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="yo" dataDxfId="99"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="J" dataDxfId="98"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="Iw" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="fy" dataDxfId="96"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="E" dataDxfId="95"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="G" dataDxfId="94"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="Axis" dataDxfId="93"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="rol" dataDxfId="92">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Section" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="An" dataDxfId="82"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="kf" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="lex" dataDxfId="80"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="ley" dataDxfId="79"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="lez" dataDxfId="78"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="rx" dataDxfId="77"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="ry" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="xo" dataDxfId="75"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="yo" dataDxfId="74"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="J" dataDxfId="73"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="Iw" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="fy" dataDxfId="71"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="E" dataDxfId="70"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="G" dataDxfId="69"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="Axis" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="rol" dataDxfId="67">
       <calculatedColumnFormula>SQRT(tblfocSglSym[[#This Row],[rx]]^2+tblfocSglSym[[#This Row],[ry]]^2+tblfocSglSym[[#This Row],[xo]]^2+tblfocSglSym[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="foz" dataDxfId="91">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="foz" dataDxfId="66">
       <calculatedColumnFormula>((tblfocSglSym[[#This Row],[G]]*tblfocSglSym[[#This Row],[J]])/(tblfocSglSym[[#This Row],[An]]*tblfocSglSym[[#This Row],[rol]]^2))*(1+((tblfocSglSym[[#This Row],[Iw]]*tblfocSglSym[[#This Row],[E]]*PI()^2)/(tblfocSglSym[[#This Row],[G]]*tblfocSglSym[[#This Row],[J]]*tblfocSglSym[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="fox_x" dataDxfId="90">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="fox_x" dataDxfId="65">
       <calculatedColumnFormula>(tblfocSglSym[[#This Row],[E]]*PI()^2)/((tblfocSglSym[[#This Row],[lex]]/tblfocSglSym[[#This Row],[rx]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="βx" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="βx" dataDxfId="64">
       <calculatedColumnFormula>1-(tblfocSglSym[[#This Row],[xo]]/tblfocSglSym[[#This Row],[rol]])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="foxz_x" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="foxz_x" dataDxfId="63">
       <calculatedColumnFormula>(1/(2*tblfocSglSym[[#This Row],[βx]]))*((tblfocSglSym[[#This Row],[fox_x]]+tblfocSglSym[[#This Row],[foz]])-SQRT((tblfocSglSym[[#This Row],[fox_x]]+tblfocSglSym[[#This Row],[foz]])^2-4*tblfocSglSym[[#This Row],[βx]]*tblfocSglSym[[#This Row],[fox_x]]*tblfocSglSym[[#This Row],[foz]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0400-00001D000000}" name="fox_y" dataDxfId="87">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0400-00001D000000}" name="fox_y" dataDxfId="62">
       <calculatedColumnFormula>(tblfocSglSym[[#This Row],[E]]*PI()^2)/((tblfocSglSym[[#This Row],[ley]]/tblfocSglSym[[#This Row],[ry]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0400-00001B000000}" name="βy" dataDxfId="86">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0400-00001B000000}" name="βy" dataDxfId="61">
       <calculatedColumnFormula>1-(tblfocSglSym[[#This Row],[yo]]/tblfocSglSym[[#This Row],[rol]])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="foxz_y" dataDxfId="85">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="foxz_y" dataDxfId="60">
       <calculatedColumnFormula>(1/(2*tblfocSglSym[[#This Row],[βy]]))*((tblfocSglSym[[#This Row],[fox_y]]+tblfocSglSym[[#This Row],[foz]])-SQRT((tblfocSglSym[[#This Row],[fox_y]]+tblfocSglSym[[#This Row],[foz]])^2-4*tblfocSglSym[[#This Row],[βy]]*tblfocSglSym[[#This Row],[fox_y]]*tblfocSglSym[[#This Row],[foz]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="foc" dataDxfId="84">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="foc" dataDxfId="59">
       <calculatedColumnFormula>IF(tblfocSglSym[[#This Row],[Axis]]="['x']",tblfocSglSym[[#This Row],[foxz_x]],tblfocSglSym[[#This Row],[foxz_y]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="λc" dataDxfId="83">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="λc" dataDxfId="58">
       <calculatedColumnFormula>SQRT(tblfocSglSym[[#This Row],[fy]]/tblfocSglSym[[#This Row],[foc]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="fn" dataDxfId="82">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="fn" dataDxfId="57">
       <calculatedColumnFormula>IF(tblfocSglSym[[#This Row],[λc]]&lt;=1.5,0.658^(tblfocSglSym[[#This Row],[λc]]^2),0.877/(tblfocSglSym[[#This Row],[λc]]^2))*tblfocSglSym[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="Nc" dataDxfId="81">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="Nc" dataDxfId="56">
       <calculatedColumnFormula>0.85*tblfocSglSym[[#This Row],[An]]*tblfocSglSym[[#This Row],[kf]]*tblfocSglSym[[#This Row],[fn]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7162,44 +7162,44 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tblfocpntsym" displayName="tblfocpntsym" ref="B2:W51" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tblfocpntsym" displayName="tblfocpntsym" ref="B2:W51" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="B2:W51" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:W59">
     <sortCondition ref="B2:B59"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Section" dataDxfId="78"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="An" dataDxfId="77"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="kf" dataDxfId="76"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="lex" dataDxfId="75"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="ley" dataDxfId="74"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0500-000013000000}" name="lez" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="rx" dataDxfId="72"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="ry" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="xo" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="yo" dataDxfId="69"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="J" dataDxfId="68"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0500-000014000000}" name="Iw" dataDxfId="67"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="fy" dataDxfId="66"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="E" dataDxfId="65"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="G" dataDxfId="64"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0500-000015000000}" name="Axis" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="rol" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Section" dataDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="An" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="kf" dataDxfId="51"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="lex" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="ley" dataDxfId="49"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0500-000013000000}" name="lez" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="rx" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="ry" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="xo" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="yo" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="J" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0500-000014000000}" name="Iw" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="fy" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="E" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="G" dataDxfId="39"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0500-000015000000}" name="Axis" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="rol" dataDxfId="37">
       <calculatedColumnFormula>SQRT(tblfocpntsym[[#This Row],[rx]]^2+tblfocpntsym[[#This Row],[ry]]^2+tblfocpntsym[[#This Row],[xo]]^2+tblfocpntsym[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="foz" dataDxfId="61">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="foz" dataDxfId="36">
       <calculatedColumnFormula>((tblfocpntsym[[#This Row],[G]]*tblfocpntsym[[#This Row],[J]])/(tblfocpntsym[[#This Row],[An]]*tblfocpntsym[[#This Row],[rol]]^2))*(1+((tblfocpntsym[[#This Row],[Iw]]*tblfocpntsym[[#This Row],[E]]*PI()^2)/(tblfocpntsym[[#This Row],[G]]*tblfocpntsym[[#This Row],[J]]*tblfocpntsym[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0500-000018000000}" name="foc" dataDxfId="60">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0500-000018000000}" name="foc" dataDxfId="35">
       <calculatedColumnFormula>tblfocpntsym[[#This Row],[foz]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="λc" dataDxfId="59">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="λc" dataDxfId="34">
       <calculatedColumnFormula>SQRT(tblfocpntsym[[#This Row],[fy]]/tblfocpntsym[[#This Row],[foc]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="fn" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="fn" dataDxfId="33">
       <calculatedColumnFormula>IF(tblfocpntsym[[#This Row],[λc]]&lt;=1.5,0.658^(tblfocpntsym[[#This Row],[λc]]^2),0.877/(tblfocpntsym[[#This Row],[λc]]^2))*tblfocpntsym[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Nc" dataDxfId="57">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Nc" dataDxfId="32">
       <calculatedColumnFormula>0.85*tblfocpntsym[[#This Row],[An]]*tblfocpntsym[[#This Row],[kf]]*tblfocpntsym[[#This Row],[fn]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7208,63 +7208,63 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tblfocunsym" displayName="tblfocunsym" ref="B2:AD57" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tblfocunsym" displayName="tblfocunsym" ref="B2:AD57" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="B2:AD57" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:AD57">
     <sortCondition ref="B2:B57"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Section" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="An" dataDxfId="53"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0600-000019000000}" name="kf" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="lex" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="ley" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="lez" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="rx" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="ry" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="xo" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="yo" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="J" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Iw" dataDxfId="43"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0600-00001A000000}" name="fy" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="E" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="G" dataDxfId="40"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0600-00001E000000}" name="Axis" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="rol" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Section" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="An" dataDxfId="28"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0600-000019000000}" name="kf" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="lex" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="ley" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="lez" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="rx" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="ry" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="xo" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="yo" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="J" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Iw" dataDxfId="18"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0600-00001A000000}" name="fy" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="E" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="G" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0600-00001E000000}" name="Axis" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="rol" dataDxfId="13">
       <calculatedColumnFormula>SQRT(tblfocunsym[[#This Row],[rx]]^2+tblfocunsym[[#This Row],[ry]]^2+tblfocunsym[[#This Row],[xo]]^2+tblfocunsym[[#This Row],[yo]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="fox" dataDxfId="37">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="fox" dataDxfId="12">
       <calculatedColumnFormula>(tblfocunsym[[#This Row],[E]]*PI()^2)/((tblfocunsym[[#This Row],[lex]]/tblfocunsym[[#This Row],[rx]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="foy" dataDxfId="36">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="foy" dataDxfId="11">
       <calculatedColumnFormula>(tblfocunsym[[#This Row],[E]]*PI()^2)/((tblfocunsym[[#This Row],[ley]]/tblfocunsym[[#This Row],[ry]])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="foz" dataDxfId="35">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="foz" dataDxfId="10">
       <calculatedColumnFormula>((tblfocunsym[[#This Row],[G]]*tblfocunsym[[#This Row],[J]])/(tblfocunsym[[#This Row],[An]]*tblfocunsym[[#This Row],[rol]]^2))*(1+((tblfocunsym[[#This Row],[Iw]]*tblfocunsym[[#This Row],[E]]*PI()^2)/(tblfocunsym[[#This Row],[G]]*tblfocunsym[[#This Row],[J]]*tblfocunsym[[#This Row],[lez]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="a" dataDxfId="34">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="a" dataDxfId="9">
       <calculatedColumnFormula>((tblfocunsym[[#This Row],[rol]]^2)-((tblfocunsym[[#This Row],[xo]]^2)*(tblfocunsym[[#This Row],[yo]]^2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0600-000013000000}" name="b" dataDxfId="33">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0600-000013000000}" name="b" dataDxfId="8">
       <calculatedColumnFormula>((tblfocunsym[[#This Row],[rol]]^2)*(tblfocunsym[[#This Row],[fox]]+tblfocunsym[[#This Row],[foy]]+tblfocunsym[[#This Row],[foz]])-((tblfocunsym[[#This Row],[foy]]*(tblfocunsym[[#This Row],[xo]]^2))+(tblfocunsym[[#This Row],[fox]]*(tblfocunsym[[#This Row],[yo]]^2))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0600-000014000000}" name="c" dataDxfId="32">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0600-000014000000}" name="c" dataDxfId="7">
       <calculatedColumnFormula>((tblfocunsym[[#This Row],[fox]]*tblfocunsym[[#This Row],[foy]])+(tblfocunsym[[#This Row],[foy]]*tblfocunsym[[#This Row],[foz]])+(tblfocunsym[[#This Row],[fox]]*tblfocunsym[[#This Row],[foz]]))*(tblfocunsym[[#This Row],[rol]]^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0600-000015000000}" name="d" dataDxfId="31">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0600-000015000000}" name="d" dataDxfId="6">
       <calculatedColumnFormula>tblfocunsym[[#This Row],[fox]]*tblfocunsym[[#This Row],[foy]]*tblfocunsym[[#This Row],[foz]]*tblfocunsym[[#This Row],[rol]]*tblfocunsym[[#This Row],[rol]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0600-000017000000}" name="eqn" dataDxfId="30">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0600-000017000000}" name="eqn" dataDxfId="5">
       <calculatedColumnFormula>tblfocunsym[[#This Row],[a]]*tblfocunsym[[#This Row],[foc]]^3-tblfocunsym[[#This Row],[b]]*tblfocunsym[[#This Row],[foc]]^2+tblfocunsym[[#This Row],[c]]*tblfocunsym[[#This Row],[foc]]-tblfocunsym[[#This Row],[d]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0600-000018000000}" name="foc" dataDxfId="29"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0600-00001B000000}" name="λc" dataDxfId="28">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0600-000018000000}" name="foc" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0600-00001B000000}" name="λc" dataDxfId="3">
       <calculatedColumnFormula>SQRT(tblfocunsym[[#This Row],[fy]]/tblfocunsym[[#This Row],[foc]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0600-00001C000000}" name="fn" dataDxfId="27">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0600-00001C000000}" name="fn" dataDxfId="2">
       <calculatedColumnFormula>IF(tblfocunsym[[#This Row],[λc]]&lt;=1.5,0.658^(tblfocunsym[[#This Row],[λc]]^2),0.877/(tblfocunsym[[#This Row],[λc]]^2))*tblfocunsym[[#This Row],[fy]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0600-00001D000000}" name="Nc" dataDxfId="26">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0600-00001D000000}" name="Nc" dataDxfId="1">
       <calculatedColumnFormula>0.85*tblfocunsym[[#This Row],[An]]*tblfocunsym[[#This Row],[kf]]*tblfocunsym[[#This Row],[fn]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7571,8 +7571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07B9FFD-D534-4711-893F-11708AF69116}">
   <dimension ref="B2:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:AA25"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7749,8 +7749,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA3" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
@@ -7831,8 +7831,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA4" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
@@ -7913,8 +7913,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA5" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
@@ -7995,8 +7995,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA6" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
@@ -8077,8 +8077,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA7" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
@@ -8159,8 +8159,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA8" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
@@ -8241,8 +8241,8 @@
         <v>1.7919999999999998E-2</v>
       </c>
       <c r="AA9" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>4480000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2688000</v>
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
@@ -8323,8 +8323,8 @@
         <v>1.536E-2</v>
       </c>
       <c r="AA10" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>3840000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2304000</v>
       </c>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
@@ -8405,8 +8405,8 @@
         <v>1.536E-2</v>
       </c>
       <c r="AA11" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>3840000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2304000</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
@@ -8487,8 +8487,8 @@
         <v>1.536E-2</v>
       </c>
       <c r="AA12" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>3840000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2304000</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
@@ -8569,8 +8569,8 @@
         <v>1.536E-2</v>
       </c>
       <c r="AA13" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>3840000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>2304000</v>
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
@@ -8651,8 +8651,8 @@
         <v>1.0320000000000001E-2</v>
       </c>
       <c r="AA14" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>2580000.0000000005</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1548000.0000000002</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
@@ -8733,8 +8733,8 @@
         <v>1.0319999999999999E-2</v>
       </c>
       <c r="AA15" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>2580000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1548000</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
@@ -8815,8 +8815,8 @@
         <v>1.0319999999999999E-2</v>
       </c>
       <c r="AA16" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>2580000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1548000</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
@@ -8897,8 +8897,8 @@
         <v>1.0319999999999999E-2</v>
       </c>
       <c r="AA17" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>2580000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1548000</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
@@ -8979,8 +8979,8 @@
         <v>7.5999999999999991E-3</v>
       </c>
       <c r="AA18" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1899999.9999999998</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1139999.9999999998</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
@@ -9061,8 +9061,8 @@
         <v>7.6E-3</v>
       </c>
       <c r="AA19" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1900000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1140000</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
@@ -9143,8 +9143,8 @@
         <v>7.6E-3</v>
       </c>
       <c r="AA20" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1900000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1140000</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
@@ -9225,8 +9225,8 @@
         <v>7.6E-3</v>
       </c>
       <c r="AA21" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1900000</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>1140000</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
@@ -9307,8 +9307,8 @@
         <v>6.5999999999999991E-3</v>
       </c>
       <c r="AA22" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1649999.9999999998</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>989999.99999999977</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
@@ -9389,8 +9389,8 @@
         <v>6.5999999999999991E-3</v>
       </c>
       <c r="AA23" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1649999.9999999998</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>989999.99999999977</v>
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.25">
@@ -9471,8 +9471,8 @@
         <v>6.5999999999999991E-3</v>
       </c>
       <c r="AA24" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1649999.9999999998</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>989999.99999999977</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
@@ -9553,8 +9553,8 @@
         <v>6.5999999999999991E-3</v>
       </c>
       <c r="AA25" s="94">
-        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]</f>
-        <v>1649999.9999999998</v>
+        <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
+        <v>989999.99999999977</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated next test for Shear
</commit_message>
<xml_diff>
--- a/tests/Excel/AS4100_5_Shear Verification.xlsx
+++ b/tests/Excel/AS4100_5_Shear Verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seank\PycharmProjects\BeamDesign\tests\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A38079-44E6-42C4-B233-3AEBBB6BF9F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0EFB1C-E99D-4352-97E7-14D8D06BBEFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Is" sheetId="11" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="256">
   <si>
     <t>J</t>
   </si>
@@ -1362,6 +1362,53 @@
       <t>u</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>v</t>
+    </r>
+  </si>
+  <si>
+    <t>limiting web slenderness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="9.35"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1382,7 +1429,7 @@
     <numFmt numFmtId="175" formatCode="0&quot; kg / m&quot;"/>
     <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1444,6 +1491,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF404041"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="9.35"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="9.35"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1542,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1593,16 +1661,46 @@
     <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="94">
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="##0.00E+00&quot; N&quot;"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="169" formatCode="##0.00E+00&quot; N&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="##0.00E+00&quot; Pa&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="##0.00E+00&quot; Pa&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000&quot; m&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="##0.00E+00&quot; N&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="##0.00E+00&quot; Pa&quot;"/>
@@ -1784,18 +1882,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="##0.00E+00&quot; Pa&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000&quot; m&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="##0.00E+00&quot; N&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="174" formatCode="##0.00E+00&quot; m²&quot;"/>
@@ -2100,9 +2186,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="##0.00E+00&quot; N&quot;"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="174" formatCode="##0.00E+00&quot; m²&quot;"/>
     </dxf>
     <dxf>
@@ -2388,9 +2471,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="tblIntegral" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="89"/>
-      <tableStyleElement type="headerRow" dxfId="88"/>
-      <tableStyleElement type="secondRowStripe" dxfId="87"/>
+      <tableStyleElement type="wholeTable" dxfId="93"/>
+      <tableStyleElement type="headerRow" dxfId="92"/>
+      <tableStyleElement type="secondRowStripe" dxfId="91"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2461,6 +2544,7 @@
       <sheetName val="UAdes"/>
       <sheetName val="RAILdim"/>
       <sheetName val="lookups"/>
+      <sheetName val="Australian Standard Section Pro"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2510,51 +2594,58 @@
       <sheetData sheetId="44"/>
       <sheetData sheetId="45"/>
       <sheetData sheetId="46"/>
+      <sheetData sheetId="47" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDDEE4D4-895F-4D98-BD2B-A1595D136FE1}" name="Table8" displayName="Table8" ref="B2:AD132" totalsRowShown="0">
-  <autoFilter ref="B2:AD132" xr:uid="{0AC04653-982D-4DB0-97C0-530DC6DA1D7C}"/>
-  <tableColumns count="29">
-    <tableColumn id="27" xr3:uid="{F0C68715-1699-4435-A336-CF305A8B079E}" name="Test_Name" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDDEE4D4-895F-4D98-BD2B-A1595D136FE1}" name="Table8" displayName="Table8" ref="B2:AF132" totalsRowShown="0">
+  <autoFilter ref="B2:AF132" xr:uid="{0AC04653-982D-4DB0-97C0-530DC6DA1D7C}"/>
+  <tableColumns count="31">
+    <tableColumn id="27" xr3:uid="{F0C68715-1699-4435-A336-CF305A8B079E}" name="Test_Name" dataDxfId="90">
       <calculatedColumnFormula>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{280EAB9D-68EA-4683-A885-68F041F7C696}" name="Section" dataDxfId="85"/>
-    <tableColumn id="29" xr3:uid="{5010BFA1-B99D-42AE-851A-22DE2AA6C466}" name="Grade" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{607776AD-1CEA-4ABA-9EBB-6E7242760D55}" name="Designation" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{8B64A8C3-F92A-47F9-96F3-AA3D2FB57C71}" name="Mass" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{C3F54EAF-B082-4E92-89A4-EB922C48C2FD}" name="Section Type" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{099E95F4-155C-46BC-9B68-09B5DC82AC9E}" name="Fabrication Type" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{603611E8-32D2-418A-B7F1-7978728F31CE}" name="d" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{8C2BF6A8-8480-4D0B-8189-8DD35F84F37A}" name="bf" dataDxfId="78"/>
-    <tableColumn id="8" xr3:uid="{AF33BA8F-44DE-4FA5-B937-5086CFDD19FF}" name="tf" dataDxfId="77"/>
-    <tableColumn id="9" xr3:uid="{688540C0-5BD0-4CE3-8BC7-7345CE0E5749}" name="tw" dataDxfId="76"/>
-    <tableColumn id="30" xr3:uid="{360F5B09-D453-4A68-ABB3-C009F0F472BF}" name="r1" dataDxfId="75"/>
-    <tableColumn id="10" xr3:uid="{1C612196-CED2-42B0-865A-D4E03216B7B7}" name="d1" dataDxfId="74"/>
-    <tableColumn id="11" xr3:uid="{4F3DA98F-ED30-4ACB-A515-75F8C0DC4843}" name="d1 / tw" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{22B64CBB-F443-44A9-9500-7B9BBDFB124B}" name="(bf - tw) / (2 × tf)" dataDxfId="72"/>
-    <tableColumn id="13" xr3:uid="{D4DF694A-4484-4C9F-9376-6A57C15AF617}" name="Ag" dataDxfId="71"/>
-    <tableColumn id="14" xr3:uid="{3724EE49-662E-4E0E-A37B-3ADE156496AD}" name="Ix" dataDxfId="70"/>
-    <tableColumn id="15" xr3:uid="{AD4648AD-343E-4A35-9246-69098C5044CC}" name="Zx" dataDxfId="69"/>
-    <tableColumn id="16" xr3:uid="{0ABFCF14-5F21-419A-9559-2CA91A10474B}" name="Sx" dataDxfId="68"/>
-    <tableColumn id="17" xr3:uid="{DC4F87E0-E5C6-4D73-A757-8F63BAF7554D}" name="rx" dataDxfId="67"/>
-    <tableColumn id="18" xr3:uid="{23E1E09C-910E-46AB-90C7-90D38D81B99E}" name="Iy" dataDxfId="66"/>
-    <tableColumn id="19" xr3:uid="{885B4339-7E0D-4B91-9FC6-5D81E2299F9C}" name="Zy" dataDxfId="65"/>
-    <tableColumn id="20" xr3:uid="{84C35746-536E-4B01-8256-14A9DCAB142B}" name="Sy" dataDxfId="64"/>
-    <tableColumn id="21" xr3:uid="{A7686837-B7AE-4BAE-88E2-6F9FAD730E01}" name="ry" dataDxfId="63"/>
-    <tableColumn id="22" xr3:uid="{767ED161-3BD1-4294-96E7-EF008EBAF27A}" name="J" dataDxfId="62"/>
-    <tableColumn id="23" xr3:uid="{4874CB8A-E902-4CEB-AEFF-C3681E512597}" name="Iw" dataDxfId="61"/>
-    <tableColumn id="26" xr3:uid="{4B448337-5DAD-4159-85BB-146825F8C228}" name="fy" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{280EAB9D-68EA-4683-A885-68F041F7C696}" name="Section" dataDxfId="89"/>
+    <tableColumn id="29" xr3:uid="{5010BFA1-B99D-42AE-851A-22DE2AA6C466}" name="Grade" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{607776AD-1CEA-4ABA-9EBB-6E7242760D55}" name="Designation" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{8B64A8C3-F92A-47F9-96F3-AA3D2FB57C71}" name="Mass" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{C3F54EAF-B082-4E92-89A4-EB922C48C2FD}" name="Section Type" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{099E95F4-155C-46BC-9B68-09B5DC82AC9E}" name="Fabrication Type" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{603611E8-32D2-418A-B7F1-7978728F31CE}" name="d" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{8C2BF6A8-8480-4D0B-8189-8DD35F84F37A}" name="bf" dataDxfId="82"/>
+    <tableColumn id="8" xr3:uid="{AF33BA8F-44DE-4FA5-B937-5086CFDD19FF}" name="tf" dataDxfId="81"/>
+    <tableColumn id="9" xr3:uid="{688540C0-5BD0-4CE3-8BC7-7345CE0E5749}" name="tw" dataDxfId="80"/>
+    <tableColumn id="30" xr3:uid="{360F5B09-D453-4A68-ABB3-C009F0F472BF}" name="r1" dataDxfId="79"/>
+    <tableColumn id="10" xr3:uid="{1C612196-CED2-42B0-865A-D4E03216B7B7}" name="d1" dataDxfId="78"/>
+    <tableColumn id="11" xr3:uid="{4F3DA98F-ED30-4ACB-A515-75F8C0DC4843}" name="d1 / tw" dataDxfId="77"/>
+    <tableColumn id="12" xr3:uid="{22B64CBB-F443-44A9-9500-7B9BBDFB124B}" name="(bf - tw) / (2 × tf)" dataDxfId="76"/>
+    <tableColumn id="13" xr3:uid="{D4DF694A-4484-4C9F-9376-6A57C15AF617}" name="Ag" dataDxfId="75"/>
+    <tableColumn id="14" xr3:uid="{3724EE49-662E-4E0E-A37B-3ADE156496AD}" name="Ix" dataDxfId="74"/>
+    <tableColumn id="15" xr3:uid="{AD4648AD-343E-4A35-9246-69098C5044CC}" name="Zx" dataDxfId="73"/>
+    <tableColumn id="16" xr3:uid="{0ABFCF14-5F21-419A-9559-2CA91A10474B}" name="Sx" dataDxfId="72"/>
+    <tableColumn id="17" xr3:uid="{DC4F87E0-E5C6-4D73-A757-8F63BAF7554D}" name="rx" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{23E1E09C-910E-46AB-90C7-90D38D81B99E}" name="Iy" dataDxfId="70"/>
+    <tableColumn id="19" xr3:uid="{885B4339-7E0D-4B91-9FC6-5D81E2299F9C}" name="Zy" dataDxfId="69"/>
+    <tableColumn id="20" xr3:uid="{84C35746-536E-4B01-8256-14A9DCAB142B}" name="Sy" dataDxfId="68"/>
+    <tableColumn id="21" xr3:uid="{A7686837-B7AE-4BAE-88E2-6F9FAD730E01}" name="ry" dataDxfId="67"/>
+    <tableColumn id="22" xr3:uid="{767ED161-3BD1-4294-96E7-EF008EBAF27A}" name="J" dataDxfId="66"/>
+    <tableColumn id="23" xr3:uid="{4874CB8A-E902-4CEB-AEFF-C3681E512597}" name="Iw" dataDxfId="65"/>
+    <tableColumn id="26" xr3:uid="{4B448337-5DAD-4159-85BB-146825F8C228}" name="fy" dataDxfId="64">
       <calculatedColumnFormula array="1">INDEX(tbllkpSteelGrades[fy],MATCH(1,(Table8[[#This Row],[Grade]]=tbllkpSteelGrades[Grade])*(Table8[[#This Row],[tw]]&lt;=tbllkpSteelGrades[Thickness]),0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{473325F2-FF03-4C75-BD12-A70F0A6AA4F1}" name="Aw" dataDxfId="59">
+    <tableColumn id="24" xr3:uid="{473325F2-FF03-4C75-BD12-A70F0A6AA4F1}" name="Aw" dataDxfId="63">
       <calculatedColumnFormula>IF(Table8[[#This Row],[Fabrication Type]]="Welded",Table8[[#This Row],[d1]],Table8[[#This Row],[d]])*Table8[[#This Row],[tw]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{98B29A8D-CA7E-401A-9966-485A14A8FF27}" name="Vyield" dataDxfId="58">
+    <tableColumn id="25" xr3:uid="{98B29A8D-CA7E-401A-9966-485A14A8FF27}" name="Vyield" dataDxfId="4">
       <calculatedColumnFormula>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="31" xr3:uid="{D2AE4FE6-949C-44C1-ABA2-0661F2AF8B79}" name="limiting web slenderness" dataDxfId="2">
+      <calculatedColumnFormula>82/SQRT(Table8[[#This Row],[fy]]/250000000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="28" xr3:uid="{350AE1F7-C8CC-4EFA-83FA-43CEF626EC3E}" name="αv" dataDxfId="3">
+      <calculatedColumnFormula>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2562,48 +2653,54 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC27F662-23F3-4692-B884-ACBE9C4BC921}" name="Table1" displayName="Table1" ref="B2:AG12" totalsRowShown="0" headerRowDxfId="57">
-  <autoFilter ref="B2:AG12" xr:uid="{159D2995-82C8-4243-A12A-2992509062CB}"/>
-  <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{BFC7DADC-5D9A-410D-8005-ABEDA04EC4E5}" name="Test Name" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EC27F662-23F3-4692-B884-ACBE9C4BC921}" name="Table1" displayName="Table1" ref="B2:AI12" totalsRowShown="0" headerRowDxfId="62">
+  <autoFilter ref="B2:AI12" xr:uid="{159D2995-82C8-4243-A12A-2992509062CB}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{BFC7DADC-5D9A-410D-8005-ABEDA04EC4E5}" name="Test Name" dataDxfId="61">
       <calculatedColumnFormula>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A68B01D6-63C3-4091-8CB2-10D8394F7045}" name="Section" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{F0C91944-5320-440C-89CC-1BCEEA04DC3A}" name="Grade" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{8BEB6DFF-49C4-4FA8-9224-463494339BF7}" name="Designation" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{AA456E27-CAB5-458A-A415-DCD765520D10}" name="Mass" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{58FBA757-33E6-4107-82A6-01450F92ECF1}" name="Section Type" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{E42F97CD-458E-4C03-887D-149CADBEE730}" name="Fabrication Type" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{30A5893B-DE67-4DB4-B63E-A74FA4F62A88}" name="d" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{DCAC7CD7-0C42-42AC-A9A3-3E6703738EA2}" name="bf" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{C94CF9A2-1DAE-4D19-BE5E-306E8BF46B88}" name="tf" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{1E144395-2B2F-424C-990F-3523916EC30D}" name="tw" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{BBC3D8A7-825A-413D-8F5B-523A8316C953}" name="r1" dataDxfId="45"/>
-    <tableColumn id="15" xr3:uid="{075B0A49-A933-463E-A295-DC05820221CD}" name="d1" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{C169B72F-E99F-4C91-8937-CA4CB5F1C0BD}" name="d1 / tw" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{EDE65130-55B8-4ED1-9338-8CF7DC57B7B0}" name="(bf - tw) / tf" dataDxfId="42"/>
-    <tableColumn id="18" xr3:uid="{B3EA4ACF-56D6-4C30-BAE3-E9AA6DECAD5B}" name="Ag" dataDxfId="41"/>
-    <tableColumn id="19" xr3:uid="{110F3BD2-1591-441D-8F2A-354835DE7C03}" name="xL" dataDxfId="40"/>
-    <tableColumn id="20" xr3:uid="{00DE344B-2B7A-4589-95FC-964370589D2F}" name="xO" dataDxfId="39"/>
-    <tableColumn id="21" xr3:uid="{74E05A20-8171-4C56-847A-4E2736645723}" name="Ix" dataDxfId="38"/>
-    <tableColumn id="22" xr3:uid="{46F05E10-2A14-4B02-8DDE-BE0422A2E11C}" name="Zx" dataDxfId="37"/>
-    <tableColumn id="23" xr3:uid="{8B5994C6-C074-4DE5-91BE-E16423FAB9D1}" name="Sx" dataDxfId="36"/>
-    <tableColumn id="24" xr3:uid="{9F69E4F9-9733-4980-9F4B-73E323CFD6C1}" name="rx" dataDxfId="35"/>
-    <tableColumn id="25" xr3:uid="{EA2F89F0-BB76-48D8-B83E-B76812070936}" name="Iy" dataDxfId="34"/>
-    <tableColumn id="26" xr3:uid="{A7187315-BF57-4454-8122-9170C02466BF}" name="ZyL" dataDxfId="33"/>
-    <tableColumn id="27" xr3:uid="{E24C8AEF-AEA2-460E-BC1B-54C7E8064ED2}" name="ZyR" dataDxfId="32"/>
-    <tableColumn id="28" xr3:uid="{CDDE43D5-2755-4C6C-98C0-89FB469561A9}" name="Sy" dataDxfId="31"/>
-    <tableColumn id="29" xr3:uid="{CC95640D-57BD-4549-8961-244E9160233E}" name="ry" dataDxfId="30"/>
-    <tableColumn id="30" xr3:uid="{4E80C201-306F-427A-B841-CC8204AC71EB}" name="J" dataDxfId="29"/>
-    <tableColumn id="31" xr3:uid="{D8BDE5DB-34D6-4AAF-94B6-6CA66EDDC4EC}" name="Iw" dataDxfId="28"/>
-    <tableColumn id="32" xr3:uid="{729B2C64-AA61-4ED8-88D9-46889D56FABC}" name="fy" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{A68B01D6-63C3-4091-8CB2-10D8394F7045}" name="Section" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{F0C91944-5320-440C-89CC-1BCEEA04DC3A}" name="Grade" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{8BEB6DFF-49C4-4FA8-9224-463494339BF7}" name="Designation" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{AA456E27-CAB5-458A-A415-DCD765520D10}" name="Mass" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{58FBA757-33E6-4107-82A6-01450F92ECF1}" name="Section Type" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{E42F97CD-458E-4C03-887D-149CADBEE730}" name="Fabrication Type" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{30A5893B-DE67-4DB4-B63E-A74FA4F62A88}" name="d" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{DCAC7CD7-0C42-42AC-A9A3-3E6703738EA2}" name="bf" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{C94CF9A2-1DAE-4D19-BE5E-306E8BF46B88}" name="tf" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{1E144395-2B2F-424C-990F-3523916EC30D}" name="tw" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{BBC3D8A7-825A-413D-8F5B-523A8316C953}" name="r1" dataDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{075B0A49-A933-463E-A295-DC05820221CD}" name="d1" dataDxfId="49"/>
+    <tableColumn id="16" xr3:uid="{C169B72F-E99F-4C91-8937-CA4CB5F1C0BD}" name="d1 / tw" dataDxfId="48"/>
+    <tableColumn id="17" xr3:uid="{EDE65130-55B8-4ED1-9338-8CF7DC57B7B0}" name="(bf - tw) / tf" dataDxfId="47"/>
+    <tableColumn id="18" xr3:uid="{B3EA4ACF-56D6-4C30-BAE3-E9AA6DECAD5B}" name="Ag" dataDxfId="46"/>
+    <tableColumn id="19" xr3:uid="{110F3BD2-1591-441D-8F2A-354835DE7C03}" name="xL" dataDxfId="45"/>
+    <tableColumn id="20" xr3:uid="{00DE344B-2B7A-4589-95FC-964370589D2F}" name="xO" dataDxfId="44"/>
+    <tableColumn id="21" xr3:uid="{74E05A20-8171-4C56-847A-4E2736645723}" name="Ix" dataDxfId="43"/>
+    <tableColumn id="22" xr3:uid="{46F05E10-2A14-4B02-8DDE-BE0422A2E11C}" name="Zx" dataDxfId="42"/>
+    <tableColumn id="23" xr3:uid="{8B5994C6-C074-4DE5-91BE-E16423FAB9D1}" name="Sx" dataDxfId="41"/>
+    <tableColumn id="24" xr3:uid="{9F69E4F9-9733-4980-9F4B-73E323CFD6C1}" name="rx" dataDxfId="40"/>
+    <tableColumn id="25" xr3:uid="{EA2F89F0-BB76-48D8-B83E-B76812070936}" name="Iy" dataDxfId="39"/>
+    <tableColumn id="26" xr3:uid="{A7187315-BF57-4454-8122-9170C02466BF}" name="ZyL" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{E24C8AEF-AEA2-460E-BC1B-54C7E8064ED2}" name="ZyR" dataDxfId="37"/>
+    <tableColumn id="28" xr3:uid="{CDDE43D5-2755-4C6C-98C0-89FB469561A9}" name="Sy" dataDxfId="36"/>
+    <tableColumn id="29" xr3:uid="{CC95640D-57BD-4549-8961-244E9160233E}" name="ry" dataDxfId="35"/>
+    <tableColumn id="30" xr3:uid="{4E80C201-306F-427A-B841-CC8204AC71EB}" name="J" dataDxfId="34"/>
+    <tableColumn id="31" xr3:uid="{D8BDE5DB-34D6-4AAF-94B6-6CA66EDDC4EC}" name="Iw" dataDxfId="33"/>
+    <tableColumn id="32" xr3:uid="{729B2C64-AA61-4ED8-88D9-46889D56FABC}" name="fy" dataDxfId="32">
       <calculatedColumnFormula array="1">INDEX(tbllkpSteelGrades[fy],MATCH(1,(Table1[[#This Row],[Grade]]=tbllkpSteelGrades[Grade])*(Table1[[#This Row],[tw]]&lt;=tbllkpSteelGrades[Thickness]),0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{F78CCC46-7A18-4959-A81C-F51FA1F9FF08}" name="Aw" dataDxfId="26">
+    <tableColumn id="33" xr3:uid="{F78CCC46-7A18-4959-A81C-F51FA1F9FF08}" name="Aw" dataDxfId="31">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Fabrication Type]]="Welded",Table1[[#This Row],[d1]],Table1[[#This Row],[d]])*Table1[[#This Row],[tw]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{EA3538CB-7B8A-4AF7-B6DC-16292E7F4F19}" name="Vyield" dataDxfId="25">
+    <tableColumn id="34" xr3:uid="{EA3538CB-7B8A-4AF7-B6DC-16292E7F4F19}" name="Vyield" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{6EFC8E23-CF2E-4C0D-BB9A-02BCA8159CF3}" name="limiting web slenderness" dataDxfId="1">
+      <calculatedColumnFormula>82/SQRT(Table1[[#This Row],[fy]]/250000000)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{3A2CC757-AD8B-4EAF-9CE0-7A223D47C931}" name="αv" dataDxfId="0">
+      <calculatedColumnFormula>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2614,31 +2711,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7CB81ECD-7B4A-4F8B-8113-71224F76D2FC}" name="Table4" displayName="Table4" ref="B2:V89" totalsRowShown="0">
   <autoFilter ref="B2:V89" xr:uid="{BA8101F0-ED77-49F7-BC18-C9D3E65708CA}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{4CA5654D-B547-49EB-AEE4-88550654C33A}" name="Test Name" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{4CA5654D-B547-49EB-AEE4-88550654C33A}" name="Test Name" dataDxfId="30">
       <calculatedColumnFormula>Table4[[#This Row],[Section]]&amp;"-"&amp;Table4[[#This Row],[Grade]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8162C8E5-B488-4140-826E-7A4F44922C08}" name="Section" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{7613563F-32CB-43B4-9CD2-B12E2A6FF2D5}" name="Grade" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C5BFAAF5-51F1-4535-980C-4B0DCD036D32}" name="Mass" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{7AAEBAA8-C99A-4F5A-88E3-88CB6960D4CA}" name="Section Type" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{B8C36499-3A13-4344-BAB0-D49EE58FE3E9}" name="Fabrication Type" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{A3848530-1431-48F2-A8A1-1A8E7187F0E4}" name="d" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{8180C5FB-397C-4385-9E2C-449435B22140}" name="t" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{721CCE1E-9271-453E-85A6-F1C3DE9BFA92}" name="d / t" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{DFEF7444-BB05-41F3-98A0-8E93565A79E0}" name="Ag" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{06548E9A-6BA5-4869-83BA-2B1ECD35C8FD}" name="I" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{04325DE9-C88D-4898-9081-69BD38E3F367}" name="Z" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{3357C355-9047-4ABB-AD18-D3E15B86E03B}" name="S" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{470CF4A9-89AA-474A-9533-AE8D1C11D912}" name="r" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{79889950-A6E3-4DDC-8073-3A8BC3FB6AD2}" name="J" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{73364D2E-305B-4F6C-B09F-DB78BE1F3A38}" name="C" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{0DA98F09-3F11-4D08-A6FC-AE92787F4FB2}" name="kf" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{716DC685-2BC9-475D-918F-7D51D96E5B00}" name="Compactness" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{1542DC57-D289-4280-A0B5-ED30B2199915}" name="Ze" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{3F052E38-FD56-42D0-85E3-1A2A4ED2525C}" name="fy" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{8162C8E5-B488-4140-826E-7A4F44922C08}" name="Section" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{7613563F-32CB-43B4-9CD2-B12E2A6FF2D5}" name="Grade" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{C5BFAAF5-51F1-4535-980C-4B0DCD036D32}" name="Mass" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{7AAEBAA8-C99A-4F5A-88E3-88CB6960D4CA}" name="Section Type" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{B8C36499-3A13-4344-BAB0-D49EE58FE3E9}" name="Fabrication Type" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{A3848530-1431-48F2-A8A1-1A8E7187F0E4}" name="d" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{8180C5FB-397C-4385-9E2C-449435B22140}" name="t" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{721CCE1E-9271-453E-85A6-F1C3DE9BFA92}" name="d / t" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{DFEF7444-BB05-41F3-98A0-8E93565A79E0}" name="Ag" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{06548E9A-6BA5-4869-83BA-2B1ECD35C8FD}" name="I" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{04325DE9-C88D-4898-9081-69BD38E3F367}" name="Z" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{3357C355-9047-4ABB-AD18-D3E15B86E03B}" name="S" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{470CF4A9-89AA-474A-9533-AE8D1C11D912}" name="r" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{79889950-A6E3-4DDC-8073-3A8BC3FB6AD2}" name="J" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{73364D2E-305B-4F6C-B09F-DB78BE1F3A38}" name="C" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{0DA98F09-3F11-4D08-A6FC-AE92787F4FB2}" name="kf" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{716DC685-2BC9-475D-918F-7D51D96E5B00}" name="Compactness" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{1542DC57-D289-4280-A0B5-ED30B2199915}" name="Ze" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{3F052E38-FD56-42D0-85E3-1A2A4ED2525C}" name="fy" dataDxfId="11">
       <calculatedColumnFormula array="1">INDEX(tbllkpSteelGrades[fy],MATCH(1,(Table4[[#This Row],[Grade]]=tbllkpSteelGrades[Grade])*(Table4[[#This Row],[t]]&lt;=tbllkpSteelGrades[Thickness]),0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{B66015BF-7FDD-4B8C-9B06-5EBF43E6C1A4}" name="Vyield" dataDxfId="0">
+    <tableColumn id="21" xr3:uid="{B66015BF-7FDD-4B8C-9B06-5EBF43E6C1A4}" name="Vyield" dataDxfId="10">
       <calculatedColumnFormula>Table4[[#This Row],[fy]]*Table4[[#This Row],[Ag]]*0.36</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2650,10 +2747,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FD922492-54C4-4564-A70A-4C52BDDF1798}" name="tbllkpSteelGrades" displayName="tbllkpSteelGrades" ref="B3:E16" totalsRowShown="0">
   <autoFilter ref="B3:E16" xr:uid="{3E6AE8C4-C748-4435-9220-6A582ED1C1D7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{523DAE2A-27B2-4510-92AE-37C4C3C1762C}" name="Grade" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{9F87EDD2-D6FD-414D-8B88-062C86BD2D39}" name="Thickness" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{102B2EDD-89A2-45B5-8609-721075A59D6E}" name="fy" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{58E14996-58E6-4334-B475-B91075D2EE2F}" name="fu" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{523DAE2A-27B2-4510-92AE-37C4C3C1762C}" name="Grade" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{9F87EDD2-D6FD-414D-8B88-062C86BD2D39}" name="Thickness" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{102B2EDD-89A2-45B5-8609-721075A59D6E}" name="fy" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{58E14996-58E6-4334-B475-B91075D2EE2F}" name="fu" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="tblIntegral" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2956,32 +3053,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07B9FFD-D534-4711-893F-11708AF69116}">
-  <dimension ref="B2:AD132"/>
+  <dimension ref="B2:AF132"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="15.85546875" customWidth="1"/>
-    <col min="23" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="15.85546875" customWidth="1"/>
-    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:32" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>55</v>
       </c>
@@ -3069,8 +3172,14 @@
       <c r="AD2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF2" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB455-300</v>
@@ -3162,8 +3271,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE3" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF3" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB423-300</v>
@@ -3255,8 +3372,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE4" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF4" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB392-300</v>
@@ -3348,8 +3473,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE5" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF5" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB342-300</v>
@@ -3441,8 +3574,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE6" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF6" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB317-300</v>
@@ -3534,8 +3675,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE7" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF7" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB278-300</v>
@@ -3627,8 +3776,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE8" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF8" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB249-300</v>
@@ -3720,8 +3877,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3225599.9999999995</v>
       </c>
-    </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE9" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF9" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB322-300</v>
@@ -3813,8 +3978,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE10" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF10" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB296-300</v>
@@ -3906,8 +4079,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE11" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF11" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB258-300</v>
@@ -3999,8 +4180,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE12" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF12" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB215-300</v>
@@ -4092,8 +4281,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE13" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF13" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB282-300</v>
@@ -4185,8 +4382,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1919520.0000000002</v>
       </c>
-    </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE14" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF14" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB257-300</v>
@@ -4278,8 +4483,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1919520</v>
       </c>
-    </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE15" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF15" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB218-300</v>
@@ -4371,8 +4584,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1919520</v>
       </c>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE16" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF16" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB175-300</v>
@@ -4464,8 +4685,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1919520</v>
       </c>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE17" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF17" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB192-300</v>
@@ -4557,8 +4786,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1413599.9999999998</v>
       </c>
-    </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE18" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF18" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.93881243856670582</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB168-300</v>
@@ -4650,8 +4887,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1413600</v>
       </c>
-    </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE19" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF19" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.93881243856670515</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB146-300</v>
@@ -4743,8 +4988,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1413600</v>
       </c>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE20" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF20" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.93881243856670515</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB122-300</v>
@@ -4836,8 +5089,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1413600</v>
       </c>
-    </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE21" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF21" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.93881243856670515</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB173-300</v>
@@ -4929,8 +5190,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1227599.9999999998</v>
       </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE22" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF22" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB150-300</v>
@@ -5022,8 +5291,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1227599.9999999998</v>
       </c>
-    </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE23" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF23" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB130-300</v>
@@ -5115,8 +5392,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1227599.9999999998</v>
       </c>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE24" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF24" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB115-300</v>
@@ -5208,8 +5493,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1227599.9999999998</v>
       </c>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE25" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>73.638173830977706</v>
+      </c>
+      <c r="AF25" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB455-400</v>
@@ -5301,8 +5594,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE26" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF26" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB423-400</v>
@@ -5394,8 +5695,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE27" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF27" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB392-400</v>
@@ -5487,8 +5796,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE28" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF28" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB342-400</v>
@@ -5580,8 +5897,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE29" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF29" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB317-400</v>
@@ -5673,8 +5998,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE30" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF30" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB278-400</v>
@@ -5766,8 +6099,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE31" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF31" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1200WB249-400</v>
@@ -5859,8 +6200,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>4085759.9999999991</v>
       </c>
-    </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE32" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF32" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.90279269602577916</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB322-400</v>
@@ -5952,8 +6301,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3502080</v>
       </c>
-    </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE33" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF33" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB296-400</v>
@@ -6045,8 +6402,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3502080</v>
       </c>
-    </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE34" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF34" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB258-400</v>
@@ -6138,8 +6503,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3502080</v>
       </c>
-    </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE35" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF35" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>1000WB215-400</v>
@@ -6231,8 +6604,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3502080</v>
       </c>
-    </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE36" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF36" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB282-400</v>
@@ -6324,8 +6705,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2476800</v>
       </c>
-    </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE37" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF37" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.81822606814494303</v>
+      </c>
+    </row>
+    <row r="38" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB257-400</v>
@@ -6417,8 +6806,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2476799.9999999995</v>
       </c>
-    </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE38" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF38" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.81822606814494325</v>
+      </c>
+    </row>
+    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB218-400</v>
@@ -6510,8 +6907,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2476799.9999999995</v>
       </c>
-    </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE39" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF39" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.81822606814494325</v>
+      </c>
+    </row>
+    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>900WB175-400</v>
@@ -6603,8 +7008,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2476799.9999999995</v>
       </c>
-    </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE40" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF40" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.81822606814494325</v>
+      </c>
+    </row>
+    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B41" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB192-400</v>
@@ -6696,8 +7109,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1823999.9999999998</v>
       </c>
-    </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE41" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF41" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.72757963988919683</v>
+      </c>
+    </row>
+    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB168-400</v>
@@ -6789,8 +7210,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1824000</v>
       </c>
-    </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE42" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF42" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.72757963988919661</v>
+      </c>
+    </row>
+    <row r="43" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB146-400</v>
@@ -6882,8 +7311,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1824000</v>
       </c>
-    </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE43" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF43" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.72757963988919661</v>
+      </c>
+    </row>
+    <row r="44" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B44" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>800WB122-400</v>
@@ -6975,8 +7412,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1824000</v>
       </c>
-    </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE44" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF44" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.72757963988919661</v>
+      </c>
+    </row>
+    <row r="45" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B45" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB173-400</v>
@@ -7068,8 +7513,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1583999.9999999998</v>
       </c>
-    </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE45" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF45" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.96476124885215842</v>
+      </c>
+    </row>
+    <row r="46" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B46" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB150-400</v>
@@ -7161,8 +7614,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1583999.9999999998</v>
       </c>
-    </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE46" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF46" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.96476124885215842</v>
+      </c>
+    </row>
+    <row r="47" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB130-400</v>
@@ -7254,8 +7715,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1583999.9999999998</v>
       </c>
-    </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE47" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF47" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.96476124885215842</v>
+      </c>
+    </row>
+    <row r="48" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>700WB115-400</v>
@@ -7347,8 +7816,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1583999.9999999998</v>
       </c>
-    </row>
-    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE48" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>64.826692033451778</v>
+      </c>
+      <c r="AF48" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>0.96476124885215842</v>
+      </c>
+    </row>
+    <row r="49" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC440-300</v>
@@ -7440,8 +7917,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2688000</v>
       </c>
-    </row>
-    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE49" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF49" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B50" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC414-300</v>
@@ -7533,8 +8018,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2150399.9999999995</v>
       </c>
-    </row>
-    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE50" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF50" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B51" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC383-300</v>
@@ -7626,8 +8119,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2150399.9999999995</v>
       </c>
-    </row>
-    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE51" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF51" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC340-300</v>
@@ -7719,8 +8220,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1890000.0000000002</v>
       </c>
-    </row>
-    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE52" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF52" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B53" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC290-300</v>
@@ -7812,8 +8321,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1620000.0000000002</v>
       </c>
-    </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE53" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF53" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC267-300</v>
@@ -7905,8 +8422,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1620000.0000000002</v>
       </c>
-    </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE54" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF54" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC228-300</v>
@@ -7998,8 +8523,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1620000.0000000002</v>
       </c>
-    </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE55" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF55" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC361-300</v>
@@ -8091,8 +8624,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2351999.9999999995</v>
       </c>
-    </row>
-    <row r="57" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE56" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF56" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B57" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC328-300</v>
@@ -8184,8 +8725,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1646400</v>
       </c>
-    </row>
-    <row r="58" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE57" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF57" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B58" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC303-300</v>
@@ -8277,8 +8826,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1646400</v>
       </c>
-    </row>
-    <row r="59" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE58" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF58" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC270-300</v>
@@ -8370,8 +8927,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1469999.9999999998</v>
       </c>
-    </row>
-    <row r="60" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE59" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF59" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC212-300</v>
@@ -8463,8 +9028,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1260000.0000000002</v>
       </c>
-    </row>
-    <row r="61" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE60" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF60" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC181-300</v>
@@ -8556,8 +9129,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1260000.0000000002</v>
       </c>
-    </row>
-    <row r="62" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE61" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF61" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC144-300</v>
@@ -8649,8 +9230,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1008000</v>
       </c>
-    </row>
-    <row r="63" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE62" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF62" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC280-300</v>
@@ -8742,8 +9331,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1293600</v>
       </c>
-    </row>
-    <row r="64" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE63" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF63" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC258-300</v>
@@ -8835,8 +9432,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1293600</v>
       </c>
-    </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE64" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF64" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC230-300</v>
@@ -8928,8 +9533,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1155000</v>
       </c>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE65" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF65" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B66" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC197-300</v>
@@ -9021,8 +9634,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>990000.00000000012</v>
       </c>
-    </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE66" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF66" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B67" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC440-400</v>
@@ -9114,8 +9735,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3456000</v>
       </c>
-    </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE67" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF67" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B68" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC414-400</v>
@@ -9207,8 +9836,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE68" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF68" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC383-400</v>
@@ -9300,8 +9937,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2764800</v>
       </c>
-    </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE69" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF69" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC340-400</v>
@@ -9393,8 +10038,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2430000</v>
       </c>
-    </row>
-    <row r="71" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE70" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF70" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC290-400</v>
@@ -9486,8 +10139,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2052000.0000000002</v>
       </c>
-    </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE71" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF71" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC267-400</v>
@@ -9579,8 +10240,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2052000.0000000002</v>
       </c>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE72" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF72" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B73" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>500WC228-400</v>
@@ -9672,8 +10341,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2052000.0000000002</v>
       </c>
-    </row>
-    <row r="74" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE73" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF73" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B74" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC361-400</v>
@@ -9765,8 +10442,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>3023999.9999999995</v>
       </c>
-    </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE74" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF74" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC328-400</v>
@@ -9858,8 +10543,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2116800</v>
       </c>
-    </row>
-    <row r="76" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE75" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF75" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B76" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC303-400</v>
@@ -9951,8 +10644,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>2116800</v>
       </c>
-    </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE76" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF76" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC270-400</v>
@@ -10044,8 +10745,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1889999.9999999995</v>
       </c>
-    </row>
-    <row r="78" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE77" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF77" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B78" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC212-400</v>
@@ -10137,8 +10846,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1596000.0000000002</v>
       </c>
-    </row>
-    <row r="79" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE78" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF78" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B79" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC181-400</v>
@@ -10230,8 +10947,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1596000.0000000002</v>
       </c>
-    </row>
-    <row r="80" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE79" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF79" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B80" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>400WC144-400</v>
@@ -10323,8 +11048,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1276800</v>
       </c>
-    </row>
-    <row r="81" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE80" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF80" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B81" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC280-400</v>
@@ -10416,8 +11149,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1663200</v>
       </c>
-    </row>
-    <row r="82" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE81" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF81" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B82" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC258-400</v>
@@ -10509,8 +11250,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1663200</v>
       </c>
-    </row>
-    <row r="83" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE82" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF82" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC230-400</v>
@@ -10602,8 +11351,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1485000.0000000002</v>
       </c>
-    </row>
-    <row r="84" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE83" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>68.333333333333343</v>
+      </c>
+      <c r="AF83" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B84" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>350WC197-400</v>
@@ -10695,8 +11452,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1254000</v>
       </c>
-    </row>
-    <row r="85" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE84" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>66.510782663612645</v>
+      </c>
+      <c r="AF84" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B85" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>610UB125-300HR</v>
@@ -10788,8 +11553,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1310904</v>
       </c>
-    </row>
-    <row r="86" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE85" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF85" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B86" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>610UB113-300HR</v>
@@ -10881,8 +11654,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1223711.9999999998</v>
       </c>
-    </row>
-    <row r="87" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE86" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF86" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B87" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>610UB101-300HR</v>
@@ -10974,8 +11755,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1225190.3999999999</v>
       </c>
-    </row>
-    <row r="88" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE87" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF87" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B88" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>530UB92.4-300HR</v>
@@ -11067,8 +11856,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1043827.2</v>
       </c>
-    </row>
-    <row r="89" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE88" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF88" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B89" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>530UB82.0-300HR</v>
@@ -11160,8 +11957,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>973209.59999999998</v>
       </c>
-    </row>
-    <row r="90" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE89" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF89" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B90" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>460UB82.1-300HR</v>
@@ -11253,8 +12058,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>874368.00000000012</v>
       </c>
-    </row>
-    <row r="91" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE90" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF90" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B91" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>460UB74.6-300HR</v>
@@ -11346,8 +12159,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>798470.40000000014</v>
       </c>
-    </row>
-    <row r="92" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE91" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF91" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>460UB67.1-300HR</v>
@@ -11439,8 +12260,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>740928.00000000012</v>
       </c>
-    </row>
-    <row r="93" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE92" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF92" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B93" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>410UB59.7-300HR</v>
@@ -11532,8 +12361,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>608025.59999999998</v>
       </c>
-    </row>
-    <row r="94" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE93" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF93" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>410UB53.7-300HR</v>
@@ -11625,8 +12462,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>588057.59999999998</v>
       </c>
-    </row>
-    <row r="95" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE94" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF94" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B95" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>360UB56.7-300HR</v>
@@ -11718,8 +12563,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>551424</v>
       </c>
-    </row>
-    <row r="96" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE95" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF95" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B96" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>360UB50.7-300HR</v>
@@ -11811,8 +12664,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>498969.59999999998</v>
       </c>
-    </row>
-    <row r="97" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE96" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF96" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B97" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>360UB44.7-300HR</v>
@@ -11904,8 +12765,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>466329.59999999998</v>
       </c>
-    </row>
-    <row r="98" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE97" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF97" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B98" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UB46.2-300HR</v>
@@ -11997,8 +12866,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>394924.79999999999</v>
       </c>
-    </row>
-    <row r="99" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE98" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF98" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B99" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UB40.4-300HR</v>
@@ -12090,8 +12967,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>356044.79999999993</v>
       </c>
-    </row>
-    <row r="100" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE99" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF99" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B100" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UB32.0-300HR</v>
@@ -12183,8 +13068,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>314688</v>
       </c>
-    </row>
-    <row r="101" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE100" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF100" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B101" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UB37.3-300HR</v>
@@ -12276,8 +13169,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>314572.79999999999</v>
       </c>
-    </row>
-    <row r="102" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE101" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF101" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B102" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UB31.4-300HR</v>
@@ -12369,8 +13270,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>295142.39999999997</v>
       </c>
-    </row>
-    <row r="103" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE102" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF102" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B103" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UB25.7-300HR</v>
@@ -12462,8 +13371,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>238080</v>
       </c>
-    </row>
-    <row r="104" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE103" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF103" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UB29.8-300HR</v>
@@ -12555,8 +13472,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>250387.19999999995</v>
       </c>
-    </row>
-    <row r="105" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE104" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF104" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UB25.4-300HR</v>
@@ -12648,8 +13573,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>226060.80000000002</v>
       </c>
-    </row>
-    <row r="106" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE105" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF105" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B106" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UB22.3-300HR</v>
@@ -12741,8 +13674,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>193920</v>
       </c>
-    </row>
-    <row r="107" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE106" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF106" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B107" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UB18.2-300HR</v>
@@ -12834,8 +13775,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>171072</v>
       </c>
-    </row>
-    <row r="108" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE107" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF107" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>180UB22.2-300HR</v>
@@ -12927,8 +13876,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>206208</v>
       </c>
-    </row>
-    <row r="109" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE108" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF108" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>180UB18.1-300HR</v>
@@ -13020,8 +13977,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>168000</v>
       </c>
-    </row>
-    <row r="110" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE109" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF109" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>180UB16.1-300HR</v>
@@ -13113,8 +14078,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>149471.99999999997</v>
       </c>
-    </row>
-    <row r="111" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE110" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF110" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B111" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>150UB18.0-300HR</v>
@@ -13206,8 +14179,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>178560</v>
       </c>
-    </row>
-    <row r="112" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE111" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF111" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B112" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>150UB14.0-300HR</v>
@@ -13299,8 +14280,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>144000</v>
       </c>
-    </row>
-    <row r="113" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE112" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF112" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B113" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UC96.8-300HR</v>
@@ -13392,8 +14381,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>585446.40000000002</v>
       </c>
-    </row>
-    <row r="114" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE113" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF113" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B114" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UC158-300HR</v>
@@ -13485,8 +14482,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>924101.99999999988</v>
       </c>
-    </row>
-    <row r="115" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE114" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF114" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B115" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UC137-300HR</v>
@@ -13578,8 +14583,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>797364</v>
       </c>
-    </row>
-    <row r="116" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE115" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF115" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B116" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UC118-300HR</v>
@@ -13671,8 +14684,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>674730</v>
       </c>
-    </row>
-    <row r="117" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE116" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF116" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B117" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UC89.5-300HR</v>
@@ -13764,8 +14785,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>524160.00000000006</v>
       </c>
-    </row>
-    <row r="118" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE117" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF117" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B118" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UC72.9-300HR</v>
@@ -13857,8 +14886,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>419404.79999999999</v>
       </c>
-    </row>
-    <row r="119" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE118" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF118" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B119" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UC59.5-300HR</v>
@@ -13950,8 +14987,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>374976</v>
       </c>
-    </row>
-    <row r="120" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE119" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF119" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B120" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UC52.2-300HR</v>
@@ -14043,8 +15088,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>316416</v>
       </c>
-    </row>
-    <row r="121" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE120" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF120" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B121" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UC46.2-300HR</v>
@@ -14136,8 +15189,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>284524.80000000005</v>
       </c>
-    </row>
-    <row r="122" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE121" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF121" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B122" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>150UC37.2-300HR</v>
@@ -14229,8 +15290,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>251942.39999999999</v>
       </c>
-    </row>
-    <row r="123" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE122" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF122" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B123" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>150UC30.0-300HR</v>
@@ -14322,8 +15391,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>200217.60000000001</v>
       </c>
-    </row>
-    <row r="124" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE123" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF123" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B124" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>150UC23.4-300HR</v>
@@ -14415,8 +15492,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>178022.39999999997</v>
       </c>
-    </row>
-    <row r="125" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE124" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF124" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B125" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>100UC14.8-300HR</v>
@@ -14508,8 +15593,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>93120</v>
       </c>
-    </row>
-    <row r="126" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE125" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF125" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B126" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UBP149-300HR</v>
@@ -14601,8 +15694,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1095192</v>
       </c>
-    </row>
-    <row r="127" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE126" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF126" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B127" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UBP146-300HR</v>
@@ -14694,8 +15795,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>1029000</v>
       </c>
-    </row>
-    <row r="128" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE127" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF127" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B128" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>200UBP122-300HR</v>
@@ -14787,8 +15896,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>966000.00000000012</v>
       </c>
-    </row>
-    <row r="129" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE128" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>77.482716966891573</v>
+      </c>
+      <c r="AF128" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B129" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UBP110-300HR</v>
@@ -14880,8 +15997,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>848232</v>
       </c>
-    </row>
-    <row r="130" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE129" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF129" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B130" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UBP84.9-300HR</v>
@@ -14973,8 +16098,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>653796</v>
       </c>
-    </row>
-    <row r="131" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE130" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF130" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B131" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>310UBP78.8-300HR</v>
@@ -15066,8 +16199,16 @@
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>597402</v>
       </c>
-    </row>
-    <row r="132" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE131" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>74.855416192372701</v>
+      </c>
+      <c r="AF131" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B132" s="15" t="str">
         <f>Table8[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table8[[#This Row],[Grade]],"0")</f>
         <v>250UBP62.6-300HR</v>
@@ -15158,6 +16299,14 @@
       <c r="AD132" s="11">
         <f>Table8[[#This Row],[Aw]]*Table8[[#This Row],[fy]]*0.6</f>
         <v>502694.39999999991</v>
+      </c>
+      <c r="AE132" s="35">
+        <f>82/SQRT(Table8[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AF132" s="36">
+        <f>IF((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])&gt;Table8[[#This Row],[limiting web slenderness]],(82/((Table8[[#This Row],[d1]]/Table8[[#This Row],[tw]])*SQRT(Table8[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -15171,15 +16320,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAB8603-8ED1-4A1F-8836-1A9DBBC119CD}">
-  <dimension ref="B2:AG12"/>
+  <dimension ref="B2:AI12"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -15201,9 +16350,11 @@
     <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:35" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="20" t="s">
         <v>131</v>
       </c>
@@ -15300,8 +16451,14 @@
       <c r="AG2" s="23" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH2" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="AI2" s="23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>380PFC-300HR</v>
@@ -15402,8 +16559,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>729600</v>
       </c>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH3" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI3" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>300PFC-300HR</v>
@@ -15504,8 +16669,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>460799.99999999994</v>
       </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH4" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI4" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>250PFC-300HR</v>
@@ -15606,8 +16779,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>384000</v>
       </c>
-    </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH5" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI5" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>230PFC-300HR</v>
@@ -15708,8 +16889,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>287040</v>
       </c>
-    </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH6" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI6" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>200PFC-300HR</v>
@@ -15810,8 +16999,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>230400.00000000003</v>
       </c>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH7" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI7" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>180PFC-300HR</v>
@@ -15912,8 +17109,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>207360</v>
       </c>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH8" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI8" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>150PFC-300HR</v>
@@ -16014,8 +17219,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>172800</v>
       </c>
-    </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH9" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI9" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>125PFC-300HR</v>
@@ -16116,8 +17329,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>112800</v>
       </c>
-    </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH10" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI10" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>100PFC-300HR</v>
@@ -16218,8 +17439,16 @@
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>80640.000000000015</v>
       </c>
-    </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AH11" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI11" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="str">
         <f>Table1[[#This Row],[Section]]&amp;"-"&amp;TEXT(Table1[[#This Row],[Grade]],"0")</f>
         <v>75PFC-300HR</v>
@@ -16319,6 +17548,14 @@
       <c r="AG12" s="11">
         <f>Table1[[#This Row],[Aw]]*Table1[[#This Row],[fy]]*0.6</f>
         <v>54720</v>
+      </c>
+      <c r="AH12" s="35">
+        <f>82/SQRT(Table1[[#This Row],[fy]]/250000000)</f>
+        <v>72.478445071621124</v>
+      </c>
+      <c r="AI12" s="36">
+        <f>IF((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])&gt;Table1[[#This Row],[limiting web slenderness]],(82/((Table1[[#This Row],[d1]]/Table1[[#This Row],[tw]])*SQRT(Table1[[#This Row],[fy]]/250000000)))^2,1)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -16333,8 +17570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7CE13B-E63F-4692-A5FE-1D44D79940EF}">
   <dimension ref="B2:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>